<commit_message>
Can fit 2D data
</commit_message>
<xml_diff>
--- a/data/heatpump.xlsx
+++ b/data/heatpump.xlsx
@@ -545,7 +545,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -616,7 +616,7 @@
         <v>328.15</v>
       </c>
       <c r="B4" s="9">
-        <v>0</v>
+        <v>2.65</v>
       </c>
       <c r="C4" s="10">
         <v>2.65</v>
@@ -636,10 +636,10 @@
         <v>333.15</v>
       </c>
       <c r="B5" s="11">
-        <v>0</v>
+        <v>2.65</v>
       </c>
       <c r="C5" s="1">
-        <v>0</v>
+        <v>2.65</v>
       </c>
       <c r="D5" s="1">
         <v>2.44</v>

</xml_diff>